<commit_message>
documenting results and testing different models on extrenal datset
</commit_message>
<xml_diff>
--- a/predictionsresnet34.xlsx
+++ b/predictionsresnet34.xlsx
@@ -31,604 +31,604 @@
     <t xml:space="preserve">Original Label</t>
   </si>
   <si>
+    <t xml:space="preserve">img01_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img01_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img01_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img01_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img02_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img02_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img02_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img02_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img03_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img03_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img03_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img03_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img04_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img04_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img04_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img04_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img05_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img05_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img05_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img05_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img06_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img06_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img06_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img06_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img07_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img07_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img07_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img07_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img08_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img08_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img08_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img08_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img09_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img09_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img09_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img09_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img10_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img10_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img10_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img10_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img11_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img11_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img11_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img11_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img12_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img12_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img12_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img12_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img13_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img13_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img13_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img13_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img14_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img14_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img14_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img14_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img15_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img15_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img15_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img15_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img16_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img16_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img16_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img16_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img17_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img17_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img17_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img17_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img18_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img18_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img18_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img18_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img19_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img19_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img19_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img19_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img20_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img20_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img20_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img20_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img21_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img21_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img21_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img21_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img22_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img22_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img22_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img22_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img23_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img23_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img23_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img23_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img24_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img24_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img24_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img24_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img25_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img25_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img25_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img25_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img26_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img26_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img26_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img26_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img27_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img27_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img27_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img27_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img28_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img28_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img28_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img28_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img29_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img29_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img29_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img29_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img30_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img30_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img30_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img30_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img31_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img31_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img31_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img31_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img32_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img32_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img32_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img32_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img33_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img33_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img33_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img33_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img34_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img34_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img34_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img34_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img35_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img35_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img35_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img35_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img36_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img36_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img36_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img36_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img37_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img37_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img37_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img37_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img38_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img38_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img38_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img38_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img39_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img39_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img39_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img39_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img40_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img40_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img40_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img40_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img41_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img41_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img41_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img41_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img42_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img42_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img42_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img42_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img43_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img43_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img43_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img43_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img44_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img44_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img44_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img44_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img45_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img45_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img45_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img45_part4.png</t>
+  </si>
+  <si>
     <t xml:space="preserve">img46_part1.png</t>
   </si>
   <si>
-    <t xml:space="preserve">img01_part2.png</t>
+    <t xml:space="preserve">img46_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img46_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img46_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img47_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img47_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img47_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img47_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img48_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img48_part2.png</t>
   </si>
   <si>
     <t xml:space="preserve">img48_part3.png</t>
   </si>
   <si>
-    <t xml:space="preserve">img32_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img12_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img43_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img12_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img25_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img26_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img19_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img07_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img03_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img06_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img38_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img10_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img47_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img45_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img44_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img03_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img31_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img13_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img13_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img15_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img46_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img43_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img04_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img27_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img17_part4.png</t>
+    <t xml:space="preserve">img48_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img49_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img49_part2.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img49_part3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img49_part4.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img50_part1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">img50_part2.png</t>
   </si>
   <si>
     <t xml:space="preserve">img50_part3.png</t>
   </si>
   <si>
-    <t xml:space="preserve">img34_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img33_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img31_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img24_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img41_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img15_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img38_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img18_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img39_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img40_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img21_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img34_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img35_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img32_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img29_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img25_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img20_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img39_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img30_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img16_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img42_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img42_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img04_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img50_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img05_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img50_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img06_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img19_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img23_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img06_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img29_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img26_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img37_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img45_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img10_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img16_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img09_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img15_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img11_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img15_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img05_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img11_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img12_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img21_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img02_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img07_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img47_part1.png</t>
-  </si>
-  <si>
     <t xml:space="preserve">img50_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img35_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img21_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img08_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img17_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img05_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img47_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img04_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img01_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img26_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img44_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img36_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img24_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img43_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img33_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img22_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img48_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img36_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img33_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img36_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img40_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img41_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img35_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img17_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img30_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img33_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img18_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img08_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img46_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img27_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img12_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img41_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img13_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img42_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img07_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img14_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img49_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img08_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img01_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img25_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img16_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img27_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img03_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img49_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img45_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img04_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img24_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img18_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img37_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img08_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img47_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img17_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img09_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img14_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img22_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img21_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img40_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img09_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img20_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img02_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img24_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img20_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img44_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img37_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img48_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img16_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img10_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img19_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img36_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img43_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img11_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img22_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img02_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img38_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img44_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img05_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img23_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img23_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img39_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img29_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img23_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img49_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img49_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img29_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img48_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img28_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img30_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img18_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img39_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img42_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img37_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img07_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img26_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img40_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img14_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img03_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img32_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img27_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img34_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img11_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img10_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img14_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img32_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img46_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img25_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img30_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img41_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img34_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img45_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img28_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img31_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img01_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img22_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img28_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img19_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img35_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img31_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img02_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img06_part4.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img13_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img20_part3.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img38_part1.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img09_part2.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">img28_part4.png</t>
   </si>
 </sst>
 </file>
@@ -744,15 +744,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C221"/>
+  <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,18 +763,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -785,7 +785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
@@ -796,18 +796,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>7</v>
       </c>
@@ -818,18 +818,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>9</v>
       </c>
@@ -840,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>10</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>11</v>
       </c>
@@ -862,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>12</v>
       </c>
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>13</v>
       </c>
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>14</v>
       </c>
@@ -895,18 +895,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>16</v>
       </c>
@@ -917,7 +917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>17</v>
       </c>
@@ -928,7 +928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>18</v>
       </c>
@@ -939,18 +939,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>20</v>
       </c>
@@ -961,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>21</v>
       </c>
@@ -972,29 +972,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>24</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>25</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>26</v>
       </c>
@@ -1027,29 +1027,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
         <v>28</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
         <v>29</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
         <v>30</v>
       </c>
@@ -1071,29 +1071,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
         <v>31</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>32</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
         <v>33</v>
       </c>
@@ -1104,18 +1104,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
         <v>35</v>
       </c>
@@ -1126,29 +1126,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>36</v>
       </c>
       <c r="B35" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>37</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
         <v>38</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>39</v>
       </c>
@@ -1170,29 +1170,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
         <v>40</v>
       </c>
       <c r="B39" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
         <v>41</v>
       </c>
       <c r="B40" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
         <v>42</v>
       </c>
@@ -1203,18 +1203,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
         <v>43</v>
       </c>
       <c r="B42" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
         <v>44</v>
       </c>
@@ -1225,29 +1225,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
         <v>45</v>
       </c>
       <c r="B44" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
         <v>46</v>
       </c>
       <c r="B45" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
         <v>47</v>
       </c>
@@ -1258,29 +1258,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
         <v>48</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
         <v>50</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
         <v>51</v>
       </c>
@@ -1302,18 +1302,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
         <v>52</v>
       </c>
       <c r="B51" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
         <v>53</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
         <v>54</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
         <v>55</v>
       </c>
@@ -1346,18 +1346,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
         <v>56</v>
       </c>
       <c r="B55" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
         <v>57</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
         <v>58</v>
       </c>
@@ -1379,18 +1379,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
         <v>59</v>
       </c>
       <c r="B58" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
         <v>60</v>
       </c>
@@ -1401,18 +1401,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
         <v>61</v>
       </c>
       <c r="B60" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
         <v>62</v>
       </c>
@@ -1423,18 +1423,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
         <v>63</v>
       </c>
       <c r="B62" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
         <v>64</v>
       </c>
@@ -1445,51 +1445,51 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
         <v>65</v>
       </c>
       <c r="B64" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
         <v>66</v>
       </c>
       <c r="B65" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
         <v>67</v>
       </c>
       <c r="B66" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
         <v>68</v>
       </c>
       <c r="B67" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
         <v>69</v>
       </c>
@@ -1500,18 +1500,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
         <v>70</v>
       </c>
       <c r="B69" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
         <v>71</v>
       </c>
@@ -1522,18 +1522,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
         <v>72</v>
       </c>
       <c r="B71" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
         <v>73</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
         <v>74</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
         <v>75</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
         <v>76</v>
       </c>
@@ -1577,29 +1577,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
         <v>77</v>
       </c>
       <c r="B76" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
         <v>78</v>
       </c>
       <c r="B77" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
         <v>79</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>80</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
         <v>81</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
         <v>82</v>
       </c>
@@ -1643,18 +1643,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>83</v>
       </c>
       <c r="B82" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>84</v>
       </c>
@@ -1665,18 +1665,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>85</v>
       </c>
       <c r="B84" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>86</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>87</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>88</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
         <v>89</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
         <v>90</v>
       </c>
@@ -1731,18 +1731,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
         <v>91</v>
       </c>
       <c r="B90" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
         <v>92</v>
       </c>
@@ -1753,40 +1753,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
         <v>93</v>
       </c>
       <c r="B92" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
         <v>94</v>
       </c>
       <c r="B93" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
         <v>95</v>
       </c>
       <c r="B94" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
         <v>96</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
         <v>97</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
         <v>98</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
         <v>99</v>
       </c>
@@ -1830,18 +1830,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>100</v>
       </c>
       <c r="B99" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>101</v>
       </c>
@@ -1852,18 +1852,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>102</v>
       </c>
       <c r="B101" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C101" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>103</v>
       </c>
@@ -1874,18 +1874,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>104</v>
       </c>
       <c r="B103" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C103" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>105</v>
       </c>
@@ -1896,29 +1896,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>106</v>
       </c>
       <c r="B105" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C105" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
         <v>107</v>
       </c>
       <c r="B106" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C106" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
         <v>108</v>
       </c>
@@ -1929,29 +1929,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
         <v>109</v>
       </c>
       <c r="B108" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C108" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>110</v>
       </c>
       <c r="B109" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C109" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
         <v>111</v>
       </c>
@@ -1962,40 +1962,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
         <v>112</v>
       </c>
       <c r="B111" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
         <v>113</v>
       </c>
       <c r="B112" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C112" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
         <v>114</v>
       </c>
       <c r="B113" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C113" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
         <v>115</v>
       </c>
@@ -2006,18 +2006,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
         <v>116</v>
       </c>
       <c r="B115" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C115" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
         <v>117</v>
       </c>
@@ -2028,18 +2028,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
         <v>118</v>
       </c>
       <c r="B117" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C117" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
         <v>119</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
         <v>120</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
         <v>121</v>
       </c>
@@ -2072,18 +2072,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
         <v>122</v>
       </c>
       <c r="B121" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C121" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
         <v>123</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
         <v>124</v>
       </c>
@@ -2105,18 +2105,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
         <v>125</v>
       </c>
       <c r="B124" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C124" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
         <v>126</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
         <v>127</v>
       </c>
@@ -2138,18 +2138,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
         <v>128</v>
       </c>
       <c r="B127" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C127" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
         <v>129</v>
       </c>
@@ -2160,18 +2160,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
         <v>130</v>
       </c>
       <c r="B129" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C129" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
         <v>131</v>
       </c>
@@ -2182,18 +2182,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
         <v>132</v>
       </c>
       <c r="B131" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C131" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
         <v>133</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
         <v>134</v>
       </c>
@@ -2215,62 +2215,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
         <v>135</v>
       </c>
       <c r="B134" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C134" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
         <v>136</v>
       </c>
       <c r="B135" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C135" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
         <v>137</v>
       </c>
       <c r="B136" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C136" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
         <v>138</v>
       </c>
       <c r="B137" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C137" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
         <v>139</v>
       </c>
       <c r="B138" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C138" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
         <v>140</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
         <v>141</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
         <v>142</v>
       </c>
@@ -2303,18 +2303,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
         <v>143</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C142" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
         <v>144</v>
       </c>
@@ -2325,18 +2325,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
         <v>145</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C144" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
         <v>146</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
         <v>147</v>
       </c>
@@ -2358,29 +2358,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>148</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C147" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
         <v>149</v>
       </c>
       <c r="B148" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C148" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
         <v>150</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
         <v>151</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
         <v>152</v>
       </c>
@@ -2413,18 +2413,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
         <v>153</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C152" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
         <v>154</v>
       </c>
@@ -2435,29 +2435,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
         <v>155</v>
       </c>
       <c r="B154" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C154" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
         <v>156</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C155" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
         <v>157</v>
       </c>
@@ -2468,62 +2468,62 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
         <v>158</v>
       </c>
       <c r="B157" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C157" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
         <v>159</v>
       </c>
       <c r="B158" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C158" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
         <v>160</v>
       </c>
       <c r="B159" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C159" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
         <v>161</v>
       </c>
       <c r="B160" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C160" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
         <v>162</v>
       </c>
       <c r="B161" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C161" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="162" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
         <v>163</v>
       </c>
@@ -2534,29 +2534,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
         <v>164</v>
       </c>
       <c r="B163" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C163" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
         <v>165</v>
       </c>
       <c r="B164" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C164" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
         <v>166</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
         <v>167</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
         <v>168</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
         <v>169</v>
       </c>
@@ -2600,7 +2600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="169" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
         <v>170</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
         <v>171</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="171" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
         <v>172</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
         <v>173</v>
       </c>
@@ -2644,62 +2644,62 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
         <v>174</v>
       </c>
       <c r="B173" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C173" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
         <v>175</v>
       </c>
       <c r="B174" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C174" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
         <v>176</v>
       </c>
       <c r="B175" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C175" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
         <v>177</v>
       </c>
       <c r="B176" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C176" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
         <v>178</v>
       </c>
       <c r="B177" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C177" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
         <v>179</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>180</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
         <v>181</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
         <v>182</v>
       </c>
@@ -2743,29 +2743,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
         <v>183</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C182" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
         <v>184</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C183" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
         <v>185</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
         <v>186</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="186" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>187</v>
       </c>
@@ -2798,18 +2798,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
         <v>188</v>
       </c>
       <c r="B187" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C187" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
         <v>189</v>
       </c>
@@ -2820,40 +2820,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
         <v>190</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C189" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
         <v>191</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C190" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
         <v>192</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C191" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="192" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
         <v>193</v>
       </c>
@@ -2864,18 +2864,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
         <v>194</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C193" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
         <v>195</v>
       </c>
@@ -2886,18 +2886,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="195" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
         <v>196</v>
       </c>
       <c r="B195" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C195" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="196" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
         <v>197</v>
       </c>
@@ -2908,51 +2908,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="197" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
         <v>198</v>
       </c>
       <c r="B197" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C197" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="198" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
         <v>199</v>
       </c>
       <c r="B198" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C198" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="199" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
         <v>200</v>
       </c>
       <c r="B199" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C199" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="200" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
         <v>201</v>
       </c>
       <c r="B200" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C200" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="201" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
         <v>202</v>
       </c>
@@ -2963,26 +2963,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>